<commit_message>
Add more tests, add code to handle scd in delivery table
</commit_message>
<xml_diff>
--- a/tests/test_input_data.xlsx
+++ b/tests/test_input_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/george.adye/Documents/git/data_model_task/tests/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{976ED64C-26AC-BF4F-BA9C-B735D7044563}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1ECC06D6-B541-4A48-803A-91CB493E1017}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="23260" windowHeight="12580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="10960" yWindow="3360" windowWidth="23260" windowHeight="12580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="in" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="53">
   <si>
     <t>OrderNumber</t>
   </si>
@@ -181,6 +181,15 @@
   </si>
   <si>
     <t>Acoustic Guitar</t>
+  </si>
+  <si>
+    <t>72 SCRIMSHIRE Lane</t>
+  </si>
+  <si>
+    <t>QUITZON, Luettgen and Waters</t>
+  </si>
+  <si>
+    <t>PO0024616-1</t>
   </si>
 </sst>
 </file>
@@ -1025,10 +1034,13 @@
   <dimension ref="A1:P13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q11" sqref="Q11"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="16" max="16" width="10.5" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
@@ -1278,7 +1290,54 @@
       </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="P6" s="1"/>
+      <c r="A6" t="s">
+        <v>52</v>
+      </c>
+      <c r="B6" t="s">
+        <v>51</v>
+      </c>
+      <c r="C6" t="s">
+        <v>33</v>
+      </c>
+      <c r="D6" t="s">
+        <v>29</v>
+      </c>
+      <c r="E6">
+        <v>2000</v>
+      </c>
+      <c r="F6">
+        <v>2</v>
+      </c>
+      <c r="G6">
+        <v>4000</v>
+      </c>
+      <c r="H6" t="s">
+        <v>20</v>
+      </c>
+      <c r="I6" t="s">
+        <v>50</v>
+      </c>
+      <c r="J6" t="s">
+        <v>35</v>
+      </c>
+      <c r="K6" t="s">
+        <v>36</v>
+      </c>
+      <c r="L6" t="s">
+        <v>24</v>
+      </c>
+      <c r="M6" t="s">
+        <v>37</v>
+      </c>
+      <c r="N6" t="s">
+        <v>28</v>
+      </c>
+      <c r="O6" t="s">
+        <v>38</v>
+      </c>
+      <c r="P6" s="1">
+        <v>44223</v>
+      </c>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.2">
       <c r="P7" s="1"/>

</xml_diff>